<commit_message>
Update 03 February  2024 - bug absen from mobile - Import validation
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_PPH.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_PPH.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
@@ -28,7 +28,25 @@
     <t xml:space="preserve">NILAI</t>
   </si>
   <si>
-    <t xml:space="preserve">PERIODE</t>
+    <t xml:space="preserve">PERIODE_PAYROLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0324230005</t>
   </si>
 </sst>
 </file>
@@ -77,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -90,6 +108,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -118,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,6 +170,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -227,10 +256,10 @@
   <dimension ref="A1:AMJ446"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.84375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.5"/>
@@ -238,7 +267,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -256,24 +285,59 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0"/>

</xml_diff>